<commit_message>
Added DEMO prefix to non-production credentials
Signed-off-by: wadeking98 <wkingnumber2@gmail.com>
</commit_message>
<xml_diff>
--- a/OCABundles/schema/bcgov-digital-trust/member-card-showcase/LSBC-OCA.xlsx
+++ b/OCABundles/schema/bcgov-digital-trust/member-card-showcase/LSBC-OCA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wadek/Documents/aries-oca-bundles/OCABundles/schema/bcgov-digital-trust/member-card-showcase/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{395DA1BE-6FA3-C043-9449-689FEF155A78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC64706F-EEAA-7F46-82AF-149266E25340}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19940" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19880" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Start Here" sheetId="1" r:id="rId1"/>
@@ -1416,7 +1416,7 @@
     <t>Y</t>
   </si>
   <si>
-    <t>Member Card</t>
+    <t>DEMO - Member Card</t>
   </si>
 </sst>
 </file>
@@ -2280,6 +2280,9 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="17" fillId="9" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2320,9 +2323,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="17" fillId="9" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -3048,28 +3048,28 @@
       <c r="D1" s="2"/>
     </row>
     <row r="2" spans="1:4" ht="34.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B2" s="73"/>
-      <c r="C2" s="73"/>
-      <c r="D2" s="73"/>
+      <c r="B2" s="74"/>
+      <c r="C2" s="74"/>
+      <c r="D2" s="74"/>
     </row>
     <row r="3" spans="1:4" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B3" s="74"/>
-      <c r="C3" s="74"/>
-      <c r="D3" s="74"/>
+      <c r="B3" s="75"/>
+      <c r="C3" s="75"/>
+      <c r="D3" s="75"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="B4" s="75"/>
-      <c r="C4" s="75"/>
-      <c r="D4" s="75"/>
+      <c r="B4" s="76"/>
+      <c r="C4" s="76"/>
+      <c r="D4" s="76"/>
     </row>
     <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="76" t="s">
+      <c r="C5" s="77" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="76"/>
+      <c r="D5" s="77"/>
     </row>
     <row r="6" spans="1:4" ht="16" x14ac:dyDescent="0.15">
       <c r="B6" s="7" t="s">
@@ -3089,10 +3089,10 @@
       <c r="B8" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="77" t="s">
+      <c r="C8" s="78" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="77"/>
+      <c r="D8" s="78"/>
     </row>
     <row r="9" spans="1:4" ht="15" x14ac:dyDescent="0.15">
       <c r="B9" s="7"/>
@@ -3108,31 +3108,31 @@
       <c r="B11" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="69"/>
-      <c r="D11" s="69"/>
+      <c r="C11" s="70"/>
+      <c r="D11" s="70"/>
     </row>
     <row r="12" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="B12" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="70"/>
-      <c r="D12" s="70"/>
+      <c r="C12" s="71"/>
+      <c r="D12" s="71"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A14" s="11"/>
-      <c r="B14" s="71" t="s">
+      <c r="B14" s="72" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="71"/>
-      <c r="D14" s="71"/>
+      <c r="C14" s="72"/>
+      <c r="D14" s="72"/>
     </row>
     <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="11"/>
-      <c r="B15" s="72" t="s">
+      <c r="B15" s="73" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="72"/>
-      <c r="D15" s="72"/>
+      <c r="C15" s="73"/>
+      <c r="D15" s="73"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -3188,11 +3188,11 @@
       <c r="D2" s="14"/>
     </row>
     <row r="3" spans="2:4" ht="93" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B3" s="81" t="s">
+      <c r="B3" s="82" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="81"/>
-      <c r="D3" s="81"/>
+      <c r="C3" s="82"/>
+      <c r="D3" s="82"/>
     </row>
     <row r="4" spans="2:4" ht="15" x14ac:dyDescent="0.15">
       <c r="B4" s="2"/>
@@ -3211,7 +3211,7 @@
       </c>
     </row>
     <row r="6" spans="2:4" ht="79.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B6" s="82" t="s">
+      <c r="B6" s="83" t="s">
         <v>16</v>
       </c>
       <c r="C6" s="17" t="s">
@@ -3222,7 +3222,7 @@
       </c>
     </row>
     <row r="7" spans="2:4" ht="48" x14ac:dyDescent="0.15">
-      <c r="B7" s="82"/>
+      <c r="B7" s="83"/>
       <c r="C7" s="19" t="s">
         <v>19</v>
       </c>
@@ -3231,7 +3231,7 @@
       </c>
     </row>
     <row r="8" spans="2:4" ht="64" x14ac:dyDescent="0.15">
-      <c r="B8" s="82"/>
+      <c r="B8" s="83"/>
       <c r="C8" s="19" t="s">
         <v>21</v>
       </c>
@@ -3240,7 +3240,7 @@
       </c>
     </row>
     <row r="9" spans="2:4" ht="48" x14ac:dyDescent="0.15">
-      <c r="B9" s="82"/>
+      <c r="B9" s="83"/>
       <c r="C9" s="19" t="s">
         <v>23</v>
       </c>
@@ -3282,7 +3282,7 @@
       </c>
     </row>
     <row r="13" spans="2:4" ht="63.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B13" s="83" t="s">
+      <c r="B13" s="84" t="s">
         <v>34</v>
       </c>
       <c r="C13" s="19" t="s">
@@ -3293,7 +3293,7 @@
       </c>
     </row>
     <row r="14" spans="2:4" ht="64" x14ac:dyDescent="0.15">
-      <c r="B14" s="83"/>
+      <c r="B14" s="84"/>
       <c r="C14" s="19" t="s">
         <v>37</v>
       </c>
@@ -3335,7 +3335,7 @@
       </c>
     </row>
     <row r="18" spans="2:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B18" s="83" t="s">
+      <c r="B18" s="84" t="s">
         <v>48</v>
       </c>
       <c r="C18" s="19" t="s">
@@ -3346,7 +3346,7 @@
       </c>
     </row>
     <row r="19" spans="2:4" ht="32" x14ac:dyDescent="0.15">
-      <c r="B19" s="83"/>
+      <c r="B19" s="84"/>
       <c r="C19" s="19" t="s">
         <v>51</v>
       </c>
@@ -3388,7 +3388,7 @@
       </c>
     </row>
     <row r="23" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B23" s="83" t="s">
+      <c r="B23" s="84" t="s">
         <v>62</v>
       </c>
       <c r="C23" s="21"/>
@@ -3397,7 +3397,7 @@
       </c>
     </row>
     <row r="24" spans="2:4" ht="32" x14ac:dyDescent="0.15">
-      <c r="B24" s="83"/>
+      <c r="B24" s="84"/>
       <c r="C24" s="19" t="s">
         <v>64</v>
       </c>
@@ -3406,7 +3406,7 @@
       </c>
     </row>
     <row r="25" spans="2:4" ht="48" x14ac:dyDescent="0.15">
-      <c r="B25" s="83"/>
+      <c r="B25" s="84"/>
       <c r="C25" s="19" t="s">
         <v>66</v>
       </c>
@@ -3415,7 +3415,7 @@
       </c>
     </row>
     <row r="26" spans="2:4" ht="64" x14ac:dyDescent="0.15">
-      <c r="B26" s="83"/>
+      <c r="B26" s="84"/>
       <c r="C26" s="19" t="s">
         <v>68</v>
       </c>
@@ -3424,7 +3424,7 @@
       </c>
     </row>
     <row r="27" spans="2:4" ht="32" x14ac:dyDescent="0.15">
-      <c r="B27" s="83"/>
+      <c r="B27" s="84"/>
       <c r="C27" s="19" t="s">
         <v>70</v>
       </c>
@@ -3433,7 +3433,7 @@
       </c>
     </row>
     <row r="28" spans="2:4" ht="80" x14ac:dyDescent="0.15">
-      <c r="B28" s="83"/>
+      <c r="B28" s="84"/>
       <c r="C28" s="19" t="s">
         <v>72</v>
       </c>
@@ -3442,7 +3442,7 @@
       </c>
     </row>
     <row r="29" spans="2:4" ht="48" x14ac:dyDescent="0.15">
-      <c r="B29" s="83"/>
+      <c r="B29" s="84"/>
       <c r="C29" s="19" t="s">
         <v>74</v>
       </c>
@@ -3451,7 +3451,7 @@
       </c>
     </row>
     <row r="30" spans="2:4" ht="48" x14ac:dyDescent="0.15">
-      <c r="B30" s="83"/>
+      <c r="B30" s="84"/>
       <c r="C30" s="19" t="s">
         <v>76</v>
       </c>
@@ -3483,18 +3483,18 @@
       <c r="D33" s="2"/>
     </row>
     <row r="34" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B34" s="78" t="s">
+      <c r="B34" s="79" t="s">
         <v>82</v>
       </c>
-      <c r="C34" s="78"/>
-      <c r="D34" s="78"/>
+      <c r="C34" s="79"/>
+      <c r="D34" s="79"/>
     </row>
     <row r="35" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B35" s="79" t="s">
+      <c r="B35" s="80" t="s">
         <v>83</v>
       </c>
-      <c r="C35" s="79"/>
-      <c r="D35" s="79"/>
+      <c r="C35" s="80"/>
+      <c r="D35" s="80"/>
     </row>
     <row r="36" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B36" s="25" t="s">
@@ -3558,16 +3558,16 @@
       <c r="D44" s="32"/>
     </row>
     <row r="45" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B45" s="80" t="s">
+      <c r="B45" s="81" t="s">
         <v>9</v>
       </c>
-      <c r="C45" s="80"/>
-      <c r="D45" s="80"/>
+      <c r="C45" s="81"/>
+      <c r="D45" s="81"/>
     </row>
     <row r="46" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B46" s="72"/>
-      <c r="C46" s="72"/>
-      <c r="D46" s="72"/>
+      <c r="B46" s="73"/>
+      <c r="C46" s="73"/>
+      <c r="D46" s="73"/>
     </row>
     <row r="47" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="48" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -36779,7 +36779,7 @@
   <dimension ref="A1:Z1003"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -36829,7 +36829,7 @@
       <c r="A4" s="61" t="s">
         <v>107</v>
       </c>
-      <c r="B4" s="84" t="s">
+      <c r="B4" s="69" t="s">
         <v>125</v>
       </c>
       <c r="C4" s="62" t="str">

</xml_diff>